<commit_message>
Update database files and enhance sale and shift management in Talinda POS. Improved error handling for user retrieval in shift and sale controllers, ensuring safe access to user information. Refactored discount calculations in the sale controller to prevent negative totals and ensure discounts do not exceed subtotals. Updated UI components for better user experience and consistency. Removed obsolete sales-related methods from product management.
</commit_message>
<xml_diff>
--- a/src/category_import_template.xlsx
+++ b/src/category_import_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>شوربة</t>
   </si>
   <si>
-    <t>عصائر طازجة</t>
-  </si>
-  <si>
     <t>كوكتيلات</t>
   </si>
   <si>
@@ -82,6 +79,12 @@
   </si>
   <si>
     <t>صواني</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عصائر فريش </t>
+  </si>
+  <si>
+    <t>الاضافات</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,7 +521,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -526,7 +529,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>14</v>
@@ -534,7 +537,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>14</v>
@@ -542,7 +545,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -550,7 +553,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>14</v>
@@ -558,7 +561,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>14</v>
@@ -566,7 +569,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -574,7 +577,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>14</v>
@@ -582,7 +585,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>14</v>
@@ -590,7 +593,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>14</v>
@@ -598,9 +601,17 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
         <v>14</v>
       </c>
     </row>

</xml_diff>